<commit_message>
Updated to address timers not sorting properly.
</commit_message>
<xml_diff>
--- a/DI_Lookup_Table.xlsx
+++ b/DI_Lookup_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB5B45F-597F-45CF-9DDF-16742D68A330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EFFC59-02A4-4AC0-9D05-D5E9D00D9806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35370" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="34080" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Server_Name</t>
   </si>
@@ -83,6 +83,24 @@
   </si>
   <si>
     <t>EDT</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_12PM</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_830PM</t>
+  </si>
+  <si>
+    <t>Haunted_Carriage_10PM</t>
+  </si>
+  <si>
+    <t>Demon_Gates_12PM</t>
+  </si>
+  <si>
+    <t>Demon_Gates_830PM</t>
+  </si>
+  <si>
+    <t>Demon_Gates_10PM</t>
   </si>
 </sst>
 </file>
@@ -434,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,9 +470,14 @@
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +508,26 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -500,7 +541,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
-Updated logic for Shadow Assembly to prevent app from crashing. -Added Wrathborne invasion.
</commit_message>
<xml_diff>
--- a/DI_Lookup_Table.xlsx
+++ b/DI_Lookup_Table.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B874D1-1DDE-4DCA-9811-7B257EF29C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5885B55D-1147-466E-9015-6AC2F00EEF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="28830" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="80">
   <si>
     <t>Server_Name</t>
   </si>
@@ -104,16 +107,193 @@
   </si>
   <si>
     <t>Ancient_Arena_930PM</t>
+  </si>
+  <si>
+    <t>Caldesann</t>
+  </si>
+  <si>
+    <t>Kanai</t>
+  </si>
+  <si>
+    <t>Eternal Crown</t>
+  </si>
+  <si>
+    <t>Deckard Cain</t>
+  </si>
+  <si>
+    <t>Zoltun Kulle</t>
+  </si>
+  <si>
+    <t>Sand Scorpions</t>
+  </si>
+  <si>
+    <t>Stormshield</t>
+  </si>
+  <si>
+    <t>Old Growth</t>
+  </si>
+  <si>
+    <t>The Soulstones</t>
+  </si>
+  <si>
+    <t>Khalim’s Will</t>
+  </si>
+  <si>
+    <t>The Gidbinn</t>
+  </si>
+  <si>
+    <t>Cult of Damnation</t>
+  </si>
+  <si>
+    <t>Purus the Decimator</t>
+  </si>
+  <si>
+    <t>Black Abyss</t>
+  </si>
+  <si>
+    <t>The Triune</t>
+  </si>
+  <si>
+    <t>Dry Steppes</t>
+  </si>
+  <si>
+    <t>Amber Blades</t>
+  </si>
+  <si>
+    <t>Halls of the Blind</t>
+  </si>
+  <si>
+    <t>Star of Azkaranth</t>
+  </si>
+  <si>
+    <t>Heart of the Oak</t>
+  </si>
+  <si>
+    <t>Crescent Moon</t>
+  </si>
+  <si>
+    <t>Call to Arms</t>
+  </si>
+  <si>
+    <t>Chains of Honor</t>
+  </si>
+  <si>
+    <t>Hand of Justice</t>
+  </si>
+  <si>
+    <t>Breath of the Dying</t>
+  </si>
+  <si>
+    <t>Pandemonium</t>
+  </si>
+  <si>
+    <t>Burning Hells</t>
+  </si>
+  <si>
+    <t>End of Days</t>
+  </si>
+  <si>
+    <t>Sin War</t>
+  </si>
+  <si>
+    <t>Prime Evils</t>
+  </si>
+  <si>
+    <t>Tree of Inifuss</t>
+  </si>
+  <si>
+    <t>Soul Siphon</t>
+  </si>
+  <si>
+    <t>Sandro the Mouth</t>
+  </si>
+  <si>
+    <t>The Malus</t>
+  </si>
+  <si>
+    <t>Iceburn Tear</t>
+  </si>
+  <si>
+    <t>Helliquary</t>
+  </si>
+  <si>
+    <t>Silver Spire</t>
+  </si>
+  <si>
+    <t>Plains of Despair</t>
+  </si>
+  <si>
+    <t>Arcane Sanctuary</t>
+  </si>
+  <si>
+    <t>The Curator</t>
+  </si>
+  <si>
+    <t>The Fallen</t>
+  </si>
+  <si>
+    <t>Risen Dead</t>
+  </si>
+  <si>
+    <t>Darkening of Tristram</t>
+  </si>
+  <si>
+    <t>Greed</t>
+  </si>
+  <si>
+    <t>The Last Vestige</t>
+  </si>
+  <si>
+    <t>Meshif</t>
+  </si>
+  <si>
+    <t>Ureh</t>
+  </si>
+  <si>
+    <t>Albrecht</t>
+  </si>
+  <si>
+    <t>Lysander</t>
+  </si>
+  <si>
+    <t>Wirt</t>
+  </si>
+  <si>
+    <t>Hadriel</t>
+  </si>
+  <si>
+    <t>Mask of Jeram</t>
+  </si>
+  <si>
+    <t>Arkaine’s Valor</t>
+  </si>
+  <si>
+    <t>Doombringer</t>
+  </si>
+  <si>
+    <t>Town Portal</t>
+  </si>
+  <si>
+    <t>Eternal Conflict</t>
+  </si>
+  <si>
+    <t>Wrathborne_Invasion_12PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,15 +635,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
@@ -481,7 +661,7 @@
     <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +713,11 @@
       <c r="Q1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -548,21 +731,812 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q1" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q59">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Added Gardens of Hope.
</commit_message>
<xml_diff>
--- a/DI_Lookup_Table.xlsx
+++ b/DI_Lookup_Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\fight\Documents\diablo_immortal_event_app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96DBC4E-D666-451D-A3DD-83B0ACF821B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027790AC-370D-4190-8799-E37763CBF4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="157">
   <si>
     <t>Server_Name</t>
   </si>
@@ -503,6 +503,12 @@
   </si>
   <si>
     <t>Withermoth</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Gardens of Hope</t>
   </si>
 </sst>
 </file>
@@ -860,33 +866,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:R123"/>
+  <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116:XFD116"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.15625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +948,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -956,7 +962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -970,7 +976,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -984,7 +990,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -1026,7 +1032,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1040,7 +1046,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1068,7 +1074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -1096,7 +1102,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1110,7 +1116,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>153</v>
       </c>
@@ -1124,7 +1130,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>133</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -1166,7 +1172,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1222,7 +1228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1236,7 +1242,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -1292,7 +1298,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1306,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>102</v>
       </c>
@@ -1348,7 +1354,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -1376,7 +1382,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1418,7 +1424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -1432,7 +1438,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1446,7 +1452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -1460,7 +1466,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -1502,7 +1508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -1516,7 +1522,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>125</v>
       </c>
@@ -1572,37 +1578,37 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B47" t="s">
-        <v>135</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>138</v>
-      </c>
-      <c r="B48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C48">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" t="s">
-        <v>141</v>
       </c>
       <c r="B49" t="s">
         <v>136</v>
@@ -1614,905 +1620,905 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>66</v>
       </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>73</v>
       </c>
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51">
-        <v>4</v>
-      </c>
-      <c r="D51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>40</v>
       </c>
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52">
-        <v>7</v>
-      </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>46</v>
       </c>
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53">
-        <v>7</v>
-      </c>
-      <c r="D53" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>42</v>
       </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54">
-        <v>7</v>
-      </c>
-      <c r="D54" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>58</v>
       </c>
-      <c r="B55" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55">
-        <v>4</v>
-      </c>
-      <c r="D55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="B56" t="s">
-        <v>135</v>
-      </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57">
-        <v>4</v>
-      </c>
-      <c r="D57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>131</v>
       </c>
-      <c r="B58" t="s">
-        <v>135</v>
-      </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>24</v>
       </c>
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59">
-        <v>7</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>32</v>
       </c>
-      <c r="B60" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60">
-        <v>7</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>113</v>
       </c>
-      <c r="B61" t="s">
-        <v>135</v>
-      </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>71</v>
       </c>
-      <c r="B62" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62">
-        <v>4</v>
-      </c>
-      <c r="D62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>74</v>
       </c>
-      <c r="B63" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63">
-        <v>4</v>
-      </c>
-      <c r="D63" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
+      <c r="B64" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>68</v>
       </c>
-      <c r="B64" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
-      </c>
-      <c r="D64" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>143</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>136</v>
       </c>
-      <c r="C65">
+      <c r="C66">
         <v>8</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>106</v>
       </c>
-      <c r="B66" t="s">
-        <v>135</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>30</v>
       </c>
-      <c r="B67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67">
-        <v>7</v>
-      </c>
-      <c r="D67" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>48</v>
       </c>
-      <c r="B68" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68">
-        <v>7</v>
-      </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>142</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>136</v>
       </c>
-      <c r="C69">
+      <c r="C70">
         <v>8</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>60</v>
       </c>
-      <c r="B70" t="s">
-        <v>14</v>
-      </c>
-      <c r="C70">
-        <v>4</v>
-      </c>
-      <c r="D70" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>52</v>
       </c>
-      <c r="B71" t="s">
-        <v>14</v>
-      </c>
-      <c r="C71">
-        <v>4</v>
-      </c>
-      <c r="D71" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>35</v>
       </c>
-      <c r="B72" t="s">
-        <v>12</v>
-      </c>
-      <c r="C72">
-        <v>7</v>
-      </c>
-      <c r="D72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>64</v>
       </c>
-      <c r="B73" t="s">
-        <v>14</v>
-      </c>
-      <c r="C73">
-        <v>4</v>
-      </c>
-      <c r="D73" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>28</v>
       </c>
-      <c r="B74" t="s">
-        <v>12</v>
-      </c>
-      <c r="C74">
-        <v>7</v>
-      </c>
-      <c r="D74" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>55</v>
       </c>
-      <c r="B75" t="s">
-        <v>14</v>
-      </c>
-      <c r="C75">
-        <v>4</v>
-      </c>
-      <c r="D75" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" t="s">
+      <c r="B76" t="s">
+        <v>14</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>101</v>
       </c>
-      <c r="B76" t="s">
-        <v>135</v>
-      </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" t="s">
+      <c r="B77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>121</v>
       </c>
-      <c r="B77" t="s">
-        <v>135</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="B78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>128</v>
       </c>
-      <c r="B78" t="s">
-        <v>135</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="B79" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>82</v>
       </c>
-      <c r="B79" t="s">
-        <v>135</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" t="s">
+      <c r="B80" t="s">
+        <v>135</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>59</v>
       </c>
-      <c r="B80" t="s">
-        <v>14</v>
-      </c>
-      <c r="C80">
-        <v>4</v>
-      </c>
-      <c r="D80" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" t="s">
+      <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>51</v>
       </c>
-      <c r="B81" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81">
-        <v>4</v>
-      </c>
-      <c r="D81" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>110</v>
       </c>
-      <c r="B82" t="s">
-        <v>135</v>
-      </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>54</v>
       </c>
-      <c r="B83" t="s">
-        <v>14</v>
-      </c>
-      <c r="C83">
-        <v>4</v>
-      </c>
-      <c r="D83" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="s">
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>41</v>
       </c>
-      <c r="B84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84">
-        <v>7</v>
-      </c>
-      <c r="D84" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>89</v>
       </c>
-      <c r="B85" t="s">
-        <v>135</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="s">
+      <c r="B86" t="s">
+        <v>135</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>29</v>
       </c>
-      <c r="B86" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86">
-        <v>7</v>
-      </c>
-      <c r="D86" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>108</v>
       </c>
-      <c r="B87" t="s">
-        <v>135</v>
-      </c>
-      <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" t="s">
+      <c r="B88" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>118</v>
       </c>
-      <c r="B88" t="s">
-        <v>135</v>
-      </c>
-      <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="B89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>127</v>
       </c>
-      <c r="B89" t="s">
-        <v>135</v>
-      </c>
-      <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="B90" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>87</v>
       </c>
-      <c r="B90" t="s">
-        <v>135</v>
-      </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-      <c r="D90" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" t="s">
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>95</v>
       </c>
-      <c r="B91" t="s">
-        <v>135</v>
-      </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" t="s">
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>99</v>
       </c>
-      <c r="B92" t="s">
-        <v>135</v>
-      </c>
-      <c r="C92">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" t="s">
+      <c r="B93" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>88</v>
       </c>
-      <c r="B93" t="s">
-        <v>135</v>
-      </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-      <c r="D93" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>86</v>
       </c>
-      <c r="B94" t="s">
-        <v>135</v>
-      </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" t="s">
+      <c r="B95" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>62</v>
       </c>
-      <c r="B95" t="s">
-        <v>14</v>
-      </c>
-      <c r="C95">
-        <v>4</v>
-      </c>
-      <c r="D95" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" t="s">
+      <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>63</v>
       </c>
-      <c r="B96" t="s">
-        <v>14</v>
-      </c>
-      <c r="C96">
-        <v>4</v>
-      </c>
-      <c r="D96" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" t="s">
+      <c r="B97" t="s">
+        <v>14</v>
+      </c>
+      <c r="C97">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>33</v>
       </c>
-      <c r="B97" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97">
-        <v>7</v>
-      </c>
-      <c r="D97" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
+        <v>12</v>
+      </c>
+      <c r="C98">
+        <v>7</v>
+      </c>
+      <c r="D98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>94</v>
       </c>
-      <c r="B98" t="s">
-        <v>135</v>
-      </c>
-      <c r="C98">
-        <v>2</v>
-      </c>
-      <c r="D98" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" t="s">
+      <c r="B99" t="s">
+        <v>135</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>67</v>
       </c>
-      <c r="B99" t="s">
-        <v>14</v>
-      </c>
-      <c r="C99">
-        <v>4</v>
-      </c>
-      <c r="D99" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" t="s">
+      <c r="B100" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>56</v>
       </c>
-      <c r="B100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C100">
-        <v>4</v>
-      </c>
-      <c r="D100" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" t="s">
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
-        <v>135</v>
-      </c>
-      <c r="C101">
-        <v>2</v>
-      </c>
-      <c r="D101" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" t="s">
+      <c r="B102" t="s">
+        <v>135</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>31</v>
       </c>
-      <c r="B102" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102">
-        <v>7</v>
-      </c>
-      <c r="D102" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>37</v>
       </c>
-      <c r="B103" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103">
-        <v>7</v>
-      </c>
-      <c r="D103" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>83</v>
       </c>
-      <c r="B104" t="s">
-        <v>135</v>
-      </c>
-      <c r="C104">
-        <v>2</v>
-      </c>
-      <c r="D104" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" t="s">
+      <c r="B105" t="s">
+        <v>135</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>90</v>
       </c>
-      <c r="B105" t="s">
-        <v>135</v>
-      </c>
-      <c r="C105">
-        <v>2</v>
-      </c>
-      <c r="D105" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
+        <v>135</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>13</v>
       </c>
-      <c r="B106" t="s">
-        <v>14</v>
-      </c>
-      <c r="C106">
-        <v>4</v>
-      </c>
-      <c r="D106" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
+        <v>14</v>
+      </c>
+      <c r="C107">
+        <v>4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>104</v>
       </c>
-      <c r="B107" t="s">
-        <v>135</v>
-      </c>
-      <c r="C107">
-        <v>2</v>
-      </c>
-      <c r="D107" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" t="s">
+      <c r="B108" t="s">
+        <v>135</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B108" t="s">
-        <v>135</v>
-      </c>
-      <c r="C108">
-        <v>2</v>
-      </c>
-      <c r="D108" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" t="s">
+      <c r="B109" t="s">
+        <v>135</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>77</v>
       </c>
-      <c r="B109" t="s">
-        <v>14</v>
-      </c>
-      <c r="C109">
-        <v>4</v>
-      </c>
-      <c r="D109" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" t="s">
+      <c r="B110" t="s">
+        <v>14</v>
+      </c>
+      <c r="C110">
+        <v>4</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>96</v>
       </c>
-      <c r="B110" t="s">
-        <v>135</v>
-      </c>
-      <c r="C110">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
+        <v>135</v>
+      </c>
+      <c r="C111">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>53</v>
       </c>
-      <c r="B111" t="s">
-        <v>14</v>
-      </c>
-      <c r="C111">
-        <v>4</v>
-      </c>
-      <c r="D111" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>69</v>
       </c>
-      <c r="B112" t="s">
-        <v>14</v>
-      </c>
-      <c r="C112">
-        <v>4</v>
-      </c>
-      <c r="D112" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" t="s">
+      <c r="B113" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113">
+        <v>4</v>
+      </c>
+      <c r="D113" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>144</v>
-      </c>
-      <c r="B113" t="s">
-        <v>136</v>
-      </c>
-      <c r="C113">
-        <v>8</v>
-      </c>
-      <c r="D113" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" t="s">
-        <v>149</v>
       </c>
       <c r="B114" t="s">
         <v>136</v>
@@ -2524,129 +2530,143 @@
         <v>151</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>149</v>
+      </c>
+      <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="C115">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>119</v>
       </c>
-      <c r="B115" t="s">
-        <v>135</v>
-      </c>
-      <c r="C115">
-        <v>2</v>
-      </c>
-      <c r="D115" t="s">
+      <c r="B116" t="s">
+        <v>135</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>72</v>
       </c>
-      <c r="B116" t="s">
-        <v>14</v>
-      </c>
-      <c r="C116">
-        <v>4</v>
-      </c>
-      <c r="D116" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" t="s">
+      <c r="B117" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117">
+        <v>4</v>
+      </c>
+      <c r="D117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>154</v>
       </c>
-      <c r="B117" t="s">
-        <v>14</v>
-      </c>
-      <c r="C117">
-        <v>4</v>
-      </c>
-      <c r="D117" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" t="s">
+      <c r="B118" t="s">
+        <v>14</v>
+      </c>
+      <c r="C118">
+        <v>4</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>105</v>
       </c>
-      <c r="B118" t="s">
-        <v>135</v>
-      </c>
-      <c r="C118">
-        <v>2</v>
-      </c>
-      <c r="D118" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" t="s">
+      <c r="B119" t="s">
+        <v>135</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>150</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B120" t="s">
         <v>136</v>
       </c>
-      <c r="C119">
+      <c r="C120">
         <v>8</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D120" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>97</v>
       </c>
-      <c r="B120" t="s">
-        <v>135</v>
-      </c>
-      <c r="C120">
-        <v>2</v>
-      </c>
-      <c r="D120" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
+        <v>135</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>139</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B122" t="s">
         <v>136</v>
       </c>
-      <c r="C121">
+      <c r="C122">
         <v>8</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>124</v>
       </c>
-      <c r="B122" t="s">
-        <v>135</v>
-      </c>
-      <c r="C122">
-        <v>2</v>
-      </c>
-      <c r="D122" t="s">
+      <c r="B123" t="s">
+        <v>135</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>27</v>
       </c>
-      <c r="B123" t="s">
-        <v>12</v>
-      </c>
-      <c r="C123">
-        <v>7</v>
-      </c>
-      <c r="D123" t="s">
+      <c r="B124" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124">
+        <v>7</v>
+      </c>
+      <c r="D124" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Fixed Wrathborne invasion timers.
</commit_message>
<xml_diff>
--- a/DI_Lookup_Table.xlsx
+++ b/DI_Lookup_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\R\diablo_immortal_event_app\DI_Timer_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fight\Documents\diablo_immortal_event_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027790AC-370D-4190-8799-E37763CBF4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FBFB38-FD31-4DBC-8AFB-0EF7D518E9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18D13C60-126E-4376-B490-60863EA4E443}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="158">
   <si>
     <t>Server_Name</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Eternal Conflict</t>
   </si>
   <si>
-    <t>Wrathborne_Invasion_12PM</t>
-  </si>
-  <si>
     <t>Dark Exile</t>
   </si>
   <si>
@@ -509,6 +506,12 @@
   </si>
   <si>
     <t>Gardens of Hope</t>
+  </si>
+  <si>
+    <t>Wrathborne_Invasion_1230PM</t>
+  </si>
+  <si>
+    <t>Wrathborne_Invasion_9PM</t>
   </si>
 </sst>
 </file>
@@ -866,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7687A13-5412-415C-B505-B9EB7AB383A0}">
-  <dimension ref="A1:R124"/>
+  <dimension ref="A1:S124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +895,7 @@
     <col min="17" max="17" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -945,10 +948,13 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="S1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -962,35 +968,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>122</v>
       </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1018,49 +1024,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" t="s">
         <v>135</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B9" t="s">
-        <v>136</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1074,21 +1080,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -1102,49 +1108,49 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1160,58 +1166,58 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19">
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,30 +1278,30 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,16 +1320,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,16 +1348,16 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,30 +1376,30 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,16 +1432,16 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,16 +1460,16 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,16 +1488,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,30 +1516,30 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C42">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
         <v>115</v>
-      </c>
-      <c r="B43" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,72 +1572,72 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
         <v>125</v>
-      </c>
-      <c r="B46" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49">
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C50">
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,16 +1726,16 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,16 +1754,16 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" t="s">
+        <v>134</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
         <v>131</v>
-      </c>
-      <c r="B59" t="s">
-        <v>135</v>
-      </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,16 +1796,16 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C62">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,30 +1852,30 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C66">
         <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1902,16 +1908,16 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70">
         <v>8</v>
       </c>
       <c r="D70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2000,58 +2006,58 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C77">
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C78">
         <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" t="s">
+        <v>134</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
         <v>128</v>
-      </c>
-      <c r="B79" t="s">
-        <v>135</v>
-      </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C80">
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,16 +2090,16 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C83">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2126,16 +2132,16 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,114 +2160,114 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
       <c r="D90" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C91">
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C92">
         <v>2</v>
       </c>
       <c r="D92" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C93">
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B94" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C94">
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B95" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,16 +2314,16 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B99" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2350,16 +2356,16 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2392,30 +2398,30 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B106" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,30 +2440,30 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C108">
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,16 +2482,16 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2518,44 +2524,44 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C114">
         <v>8</v>
       </c>
       <c r="D114" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C115">
         <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2574,7 +2580,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B118" t="s">
         <v>14</v>
@@ -2588,72 +2594,72 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C120">
         <v>8</v>
       </c>
       <c r="D120" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B121" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C122">
         <v>8</v>
       </c>
       <c r="D122" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B123" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>